<commit_message>
editing for player table import
</commit_message>
<xml_diff>
--- a/data/old/team_names.xlsx
+++ b/data/old/team_names.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattw\Documents\ff_shiny_app\ff_app\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattw\Documents\ff_shiny_app\ff_app\data\old\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36D5E62-D56A-4E13-B2CF-DBD1551DBF59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A777FF1F-DC19-4554-ACD2-EDB725162A47}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{EF31F54B-043B-4B28-8153-23D79D0673AD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="120">
   <si>
     <t>New England Patriots</t>
   </si>
@@ -390,6 +390,9 @@
   </si>
   <si>
     <t>afc_south</t>
+  </si>
+  <si>
+    <t>team_id</t>
   </si>
 </sst>
 </file>
@@ -445,13 +448,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -768,683 +777,782 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AAC5F7E-09C3-475F-A1B9-3DF3FC47BB96}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>62</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>53</v>
       </c>
       <c r="C2" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>109</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>50</v>
       </c>
       <c r="C3" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>109</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>110</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>55</v>
       </c>
       <c r="C5" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>110</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>54</v>
       </c>
       <c r="C6" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>109</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>60</v>
       </c>
       <c r="C7" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>109</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>45</v>
       </c>
       <c r="C8" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>110</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>28</v>
-      </c>
-      <c r="B9" t="s">
-        <v>59</v>
       </c>
       <c r="C9" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>110</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>32</v>
       </c>
       <c r="C10" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>109</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
         <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>47</v>
       </c>
       <c r="C11" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>110</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>44</v>
       </c>
       <c r="C12" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>109</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>1</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>49</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>109</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>21</v>
-      </c>
-      <c r="B14" t="s">
-        <v>43</v>
       </c>
       <c r="C14" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>110</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
         <v>23</v>
-      </c>
-      <c r="B15" t="s">
-        <v>41</v>
       </c>
       <c r="C15" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>110</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>27</v>
-      </c>
-      <c r="B16" t="s">
-        <v>37</v>
       </c>
       <c r="C16" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>110</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+    <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>14</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>33</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>110</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+    <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" t="s">
+        <v>104</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F18" t="s">
+        <v>110</v>
+      </c>
+      <c r="G18" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
         <v>13</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C19" t="s">
         <v>39</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D19" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F19" t="s">
         <v>110</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G19" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>16</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C20" t="s">
         <v>56</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D20" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F20" t="s">
         <v>109</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G20" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+    <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
         <v>29</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C21" t="s">
         <v>57</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D21" t="s">
         <v>57</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F21" t="s">
         <v>110</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G21" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+    <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
         <v>4</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C22" t="s">
         <v>34</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D22" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F22" t="s">
         <v>109</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G22" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+    <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
         <v>0</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C23" t="s">
         <v>38</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D23" t="s">
         <v>64</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F23" t="s">
         <v>110</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G23" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+    <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
         <v>19</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C24" t="s">
         <v>46</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D24" t="s">
         <v>66</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F24" t="s">
         <v>109</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G24" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
         <v>26</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C25" t="s">
         <v>48</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D25" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F25" t="s">
         <v>109</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G25" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
         <v>7</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C26" t="s">
         <v>51</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D26" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F26" t="s">
         <v>110</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G26" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+    <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
         <v>15</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C27" t="s">
         <v>40</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D27" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F27" t="s">
         <v>109</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G27" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+    <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
         <v>25</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C28" t="s">
         <v>58</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D28" t="s">
         <v>58</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F28" t="s">
         <v>110</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G28" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+    <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
         <v>9</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C29" t="s">
         <v>52</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D29" t="s">
         <v>67</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F29" t="s">
         <v>109</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G29" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+    <row r="30" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
         <v>10</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C30" t="s">
         <v>35</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D30" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F30" t="s">
         <v>109</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G30" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
         <v>24</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C31" t="s">
         <v>61</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D31" t="s">
         <v>69</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="E31" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F31" t="s">
         <v>109</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G31" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
         <v>5</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C32" t="s">
         <v>36</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D32" t="s">
         <v>36</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="E32" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F32" t="s">
         <v>110</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G32" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
         <v>106</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C33" t="s">
         <v>42</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D33" t="s">
         <v>42</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="E33" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F33" t="s">
         <v>109</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G33" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>103</v>
-      </c>
-      <c r="B33" t="s">
-        <v>105</v>
-      </c>
-      <c r="C33" t="s">
-        <v>104</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E33" t="s">
-        <v>110</v>
-      </c>
-      <c r="F33" t="s">
-        <v>112</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:C32">
-    <sortCondition ref="C2"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G33">
+    <sortCondition ref="B1:B33"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>